<commit_message>
feat(Salary): export salary template go to bank
</commit_message>
<xml_diff>
--- a/src/storage/app/excel-exporter/templates/salary_payment_template.xlsx
+++ b/src/storage/app/excel-exporter/templates/salary_payment_template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t xml:space="preserve">CÔNG TY TNHH DỊCH VỤ CHẤN THANH</t>
   </si>
@@ -59,9 +59,6 @@
   </si>
   <si>
     <t xml:space="preserve">GIÁM ĐỐC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NGUYỄN HUỲNH THU TRÚC</t>
   </si>
 </sst>
 </file>
@@ -270,10 +267,10 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.83203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.9"/>
@@ -788,9 +785,7 @@
     <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
-      <c r="C18" s="17" t="s">
-        <v>13</v>
-      </c>
+      <c r="C18" s="17"/>
       <c r="D18" s="18"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>

</xml_diff>